<commit_message>
fixing ACC for slide, calendar and dropdown
</commit_message>
<xml_diff>
--- a/Data Binding Daftar.xlsx
+++ b/Data Binding Daftar.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Videos\Project in ACC - ACCOne MOBILE 2832019\Project in ACC - ACCOne MOBILE 2832019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomyhidayat/Documents/OneDrive/comp/ACC/katalon_sourcecode/acc-implementation/accone-mobile/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997B536F-D4C6-BC4C-A3CA-631CF510FC95}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,23 +396,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.125" customWidth="1"/>
-    <col min="5" max="5" width="21.375" customWidth="1"/>
-    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -439,7 +440,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>87824121996</v>
+        <v>87824121997</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -451,7 +452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -459,7 +460,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>87824121996</v>
+        <v>87824121997</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -471,13 +472,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
-        <v>87824121996</v>
+        <v>87824121997</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -486,7 +487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -494,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>87824121996</v>
+        <v>87824121997</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -508,9 +509,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>